<commit_message>
chore: better option names
</commit_message>
<xml_diff>
--- a/test/resources/datasets/header.xlsx
+++ b/test/resources/datasets/header.xlsx
@@ -26,7 +26,7 @@
     <t xml:space="preserve">first page does not contain the data</t>
   </si>
   <si>
-    <t xml:space="preserve">second page has a header that must be ignores</t>
+    <t xml:space="preserve">second page has a header that must be ignored</t>
   </si>
   <si>
     <t xml:space="preserve">col1</t>
@@ -53,6 +53,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -112,8 +113,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -249,7 +254,7 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -272,29 +277,29 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>